<commit_message>
Added FRA and Futures Excel Pricing Workbooks
</commit_message>
<xml_diff>
--- a/03 Products & Pricing/09 Futures/Futures.xlsx
+++ b/03 Products & Pricing/09 Futures/Futures.xlsx
@@ -1,16 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\03 Products &amp; Pricing\09 Futures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2A7C7-C648-42AF-B059-0DB0D4A0CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Futures" sheetId="1" r:id="rId1"/>
-    <sheet name="Tickers" sheetId="2" r:id="rId2"/>
+    <sheet name="Futures Tickers" sheetId="2" r:id="rId1"/>
+    <sheet name="Compound Interest" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -195,7 +213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -437,6 +455,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,7 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,11 +554,107 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29087</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6724650" y="2266950"/>
+          <a:ext cx="3667637" cy="1629002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>124693</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="190500"/>
+          <a:ext cx="6220693" cy="1743318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -554,7 +668,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -610,7 +730,7 @@
                     <m:sSubPr>
                       <m:ctrlPr>
                         <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
                       </m:ctrlPr>
                     </m:sSubPr>
@@ -655,7 +775,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -673,7 +793,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="Cambria Math"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -708,7 +828,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="Cambria Math"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -735,7 +855,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -750,7 +870,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="Cambria Math"/>
+                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -765,7 +885,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="Cambria Math"/>
+                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -838,7 +958,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -853,7 +973,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="Cambria Math"/>
+                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -868,7 +988,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="Cambria Math"/>
+                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -974,7 +1094,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -989,7 +1109,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="Cambria Math"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -1021,7 +1141,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="Cambria Math"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1054,7 +1174,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1365,7 +1485,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1421,7 +1547,7 @@
                     <m:sSubPr>
                       <m:ctrlPr>
                         <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
                       </m:ctrlPr>
                     </m:sSubPr>
@@ -1465,7 +1591,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -1482,7 +1608,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="Cambria Math"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -1500,7 +1626,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="Cambria Math"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1533,7 +1659,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1548,7 +1674,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="Cambria Math"/>
+                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1563,7 +1689,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="Cambria Math"/>
+                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1636,7 +1762,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -1651,7 +1777,7 @@
                                             <a:schemeClr val="tx1"/>
                                           </a:solidFill>
                                           <a:effectLst/>
-                                          <a:latin typeface="Cambria Math"/>
+                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:ea typeface="+mn-ea"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
@@ -1666,7 +1792,7 @@
                                                 <a:schemeClr val="tx1"/>
                                               </a:solidFill>
                                               <a:effectLst/>
-                                              <a:latin typeface="Cambria Math"/>
+                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                               <a:ea typeface="+mn-ea"/>
                                               <a:cs typeface="+mn-cs"/>
                                             </a:rPr>
@@ -1736,7 +1862,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="Cambria Math"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -1769,7 +1895,7 @@
                                     <a:schemeClr val="tx1"/>
                                   </a:solidFill>
                                   <a:effectLst/>
-                                  <a:latin typeface="Cambria Math"/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                   <a:ea typeface="+mn-ea"/>
                                   <a:cs typeface="+mn-cs"/>
                                 </a:rPr>
@@ -1961,87 +2087,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>29087</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85952</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6724650" y="2266950"/>
-          <a:ext cx="3667637" cy="1629002"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>124693</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>9768</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6705600" y="190500"/>
-          <a:ext cx="6220693" cy="1743318"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2085,7 +2130,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2118,9 +2163,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2153,6 +2215,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2328,354 +2407,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G24"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="5" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <f ca="1">2*RAND()*$D$2</f>
-        <v>5.6933979636380645</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" ref="E5:E14" ca="1" si="0">(1+C5/360*D5/100)</f>
-        <v>1.0001581499434344</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" ref="D6:D14" ca="1" si="1">2*RAND()*$D$2</f>
-        <v>7.047577912578963</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0001957660531271</v>
-      </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0047567166484193</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0001390210199068</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.5000022147784158</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0000972222837439</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.349500512787948</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0007791250427323</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.1149097877754226</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0001698586052159</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6710642152853428</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.000129751783758</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.51240305495132032</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0000142334181932</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.5308765791423049</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0002091910160873</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.4321851250465176</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0004526820937538</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="3">
-        <f>SUM(C5:C15)</f>
-        <v>14</v>
-      </c>
-      <c r="D17" s="6">
-        <f ca="1">SUMPRODUCT(D5:D14,C5:C14)/C17</f>
-        <v>6.0300032398786891</v>
-      </c>
-      <c r="E17" s="6">
-        <f ca="1">(PRODUCT(E5:E15)-1)*(360/C17)*100</f>
-        <v>6.0357988222738967</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="6">
-        <f ca="1">100-D17</f>
-        <v>93.969996760121305</v>
-      </c>
-      <c r="E23" s="6">
-        <f ca="1">100-E17</f>
-        <v>93.964201177726096</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="29" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="25" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="34">
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="35">
         <v>23</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="36"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
+    </row>
+    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
@@ -2685,13 +2480,13 @@
       <c r="D8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2702,13 +2497,13 @@
         <f t="shared" ref="D9:D12" si="0">B9&amp;C9</f>
         <v>EDH3</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2719,13 +2514,13 @@
         <f t="shared" si="0"/>
         <v>EDM3</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2736,13 +2531,13 @@
         <f t="shared" si="0"/>
         <v>EDU3</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
@@ -2753,67 +2548,67 @@
         <f t="shared" si="0"/>
         <v>EDZ3</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="19" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="29" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="34">
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="35">
         <v>3</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="36"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -2839,4 +2634,288 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="5" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <f ca="1">2*RAND()*$D$2</f>
+        <v>8.3252073393724153</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" ref="E5:E14" ca="1" si="0">(1+C5/360*D5/100)</f>
+        <v>1.0002312557594271</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D14" ca="1" si="1">2*RAND()*$D$2</f>
+        <v>0.28066823268662389</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0000077963397969</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.7901012941726098</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0002163917026159</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.9830141876263507</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0002773059496564</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.7693685519338835</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0007307807126611</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6939577381174225</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0002414988260588</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.3116370531066268</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0001753232514752</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.1034367176890729</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0002528732421581</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.1397890813153619</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0001427719189255</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16712345439670484</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.000013926954533</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="3">
+        <f>SUM(C5:C15)</f>
+        <v>14</v>
+      </c>
+      <c r="D17" s="6">
+        <f ca="1">SUMPRODUCT(D5:D14,C5:C14)/C17</f>
+        <v>5.8883776902198752</v>
+      </c>
+      <c r="E17" s="6">
+        <f ca="1">(PRODUCT(E5:E15)-1)*(360/C17)*100</f>
+        <v>5.8939848959940839</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="6">
+        <f ca="1">100-D17</f>
+        <v>94.111622309780131</v>
+      </c>
+      <c r="E23" s="6">
+        <f ca="1">100-E17</f>
+        <v>94.10601510400592</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating Futures and FRA pricing workbooks
</commit_message>
<xml_diff>
--- a/03 Products & Pricing/09 Futures/Futures.xlsx
+++ b/03 Products & Pricing/09 Futures/Futures.xlsx
@@ -8,14 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\03 Products &amp; Pricing\09 Futures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2A7C7-C648-42AF-B059-0DB0D4A0CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C920BD15-47E9-4396-8D92-289DBF1F5300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Futures Tickers" sheetId="2" r:id="rId1"/>
-    <sheet name="Compound Interest" sheetId="1" r:id="rId2"/>
+    <sheet name="Futures Prices &amp; Margin" sheetId="3" r:id="rId1"/>
+    <sheet name="Futures Tickers" sheetId="2" r:id="rId2"/>
+    <sheet name="USD 3M SOFR Futures" sheetId="4" r:id="rId3"/>
+    <sheet name="Compound Interest" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="ContractSize">'Futures Prices &amp; Margin'!$C$4</definedName>
+    <definedName name="FuturesTable">'Futures Prices &amp; Margin'!$I$8:$Q$15</definedName>
+    <definedName name="FuturesTickers">'Futures Prices &amp; Margin'!$I$8:$I$15</definedName>
+    <definedName name="Ticker">'Futures Prices &amp; Margin'!$C$2</definedName>
+    <definedName name="TickValue">'Futures Prices &amp; Margin'!$C$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>r</t>
   </si>
@@ -209,16 +218,268 @@
   <si>
     <t>Eurodollar Futures SEP-2023</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Price (bps)</t>
+  </si>
+  <si>
+    <t>TickValue</t>
+  </si>
+  <si>
+    <t>ContractSize</t>
+  </si>
+  <si>
+    <t>+/-</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>Contract Size</t>
+  </si>
+  <si>
+    <t>USD 3M LIBOR Futures</t>
+  </si>
+  <si>
+    <t>USD 1M SOFR Futures</t>
+  </si>
+  <si>
+    <t>USD 3M SOFR Futures</t>
+  </si>
+  <si>
+    <t>GBP 3M LIBOR Futures</t>
+  </si>
+  <si>
+    <t>GBP 3M SONIA Futures</t>
+  </si>
+  <si>
+    <t>EUR 3M LIBOR Futures</t>
+  </si>
+  <si>
+    <t>EUR 1M ESTR Futures</t>
+  </si>
+  <si>
+    <t>JPY 3M TIBOR Futures</t>
+  </si>
+  <si>
+    <t>SO3</t>
+  </si>
+  <si>
+    <t>CCY</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>EON</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.cmegroup.com/markets/interest-rates/stirs/three-month-sofr.quotes.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>SOFR Settlement Calculation</t>
+  </si>
+  <si>
+    <t>https://www.cmegroup.com/education/files/sofr-futures-settlement-calculation-methodologies.pdf</t>
+  </si>
+  <si>
+    <t>Term Rate</t>
+  </si>
+  <si>
+    <t>Excellent Futures Guide</t>
+  </si>
+  <si>
+    <t>http://www.yieldcurve.com/Mktresearch/LearningCurve/InterestRateFutures.pdf</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Tick Value Calculation</t>
+  </si>
+  <si>
+    <t>Contract Period</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>Net Margin</t>
+  </si>
+  <si>
+    <t>Futures Ticker</t>
+  </si>
+  <si>
+    <t>Start Price</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>e.g. Tick Value(ED) = 1,000,000 * 0.25 * 0.01%</t>
+  </si>
+  <si>
+    <r>
+      <t>Tick Value = Contract Size x Contract Period</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> x 1 bps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tick Value</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tick value per basis point (bps)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Contract period in years is computed using 30/360 daycount basis to give a regular constant contract periods</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="ddd\,\ d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +539,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,8 +625,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -419,12 +740,236 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,6 +1087,157 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -550,6 +1246,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -655,6 +1356,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>77263</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>91892</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB666CE9-D4D2-345A-74C9-023A741DAE81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="182880"/>
+          <a:ext cx="12269263" cy="5212532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2407,10 +3157,699 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF2E4AC-8323-409E-8AF9-D65640EDC1C6}">
+  <dimension ref="B2:T27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="44"/>
+    <col min="2" max="2" width="16.33203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="8.88671875" style="44"/>
+    <col min="14" max="14" width="15" style="44" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="44" customWidth="1"/>
+    <col min="16" max="17" width="12.77734375" style="44" customWidth="1"/>
+    <col min="18" max="19" width="8.88671875" style="44"/>
+    <col min="20" max="20" width="15" style="44" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B2" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="I2" s="78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B3" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="42" t="str">
+        <f>VLOOKUP(Ticker,FuturesTable,2,0)</f>
+        <v>USD 3M LIBOR Futures</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="45">
+        <f>VLOOKUP(Ticker,FuturesTable,6,0)</f>
+        <v>1000000</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="I4" s="44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="46">
+        <f>VLOOKUP(Ticker,FuturesTable,8,0)</f>
+        <v>25</v>
+      </c>
+      <c r="D5" s="43"/>
+      <c r="I5" s="44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+    </row>
+    <row r="7" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" s="45"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="49">
+        <v>37062</v>
+      </c>
+      <c r="C8" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="D8" s="45">
+        <v>9900</v>
+      </c>
+      <c r="E8" s="45">
+        <f t="shared" ref="E8:E21" si="0">D8-D9</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="51">
+        <f t="shared" ref="F8:F15" si="1">TickValue*E8</f>
+        <v>25</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="69">
+        <v>1000000</v>
+      </c>
+      <c r="O8" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="58">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="T8" s="45"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="49">
+        <v>37061</v>
+      </c>
+      <c r="C9" s="50">
+        <v>0.9899</v>
+      </c>
+      <c r="D9" s="45">
+        <v>9899</v>
+      </c>
+      <c r="E9" s="45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="45">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="79">
+        <v>5000000</v>
+      </c>
+      <c r="O9" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="P9" s="61">
+        <v>41.67</v>
+      </c>
+      <c r="Q9" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="45"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="49">
+        <v>37060</v>
+      </c>
+      <c r="C10" s="50">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="D10" s="45">
+        <v>9897</v>
+      </c>
+      <c r="E10" s="45">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F10" s="45">
+        <f t="shared" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="I10" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="85">
+        <v>1000000</v>
+      </c>
+      <c r="O10" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="87">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="45"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="49">
+        <v>37057</v>
+      </c>
+      <c r="C11" s="50">
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="D11" s="45">
+        <v>9898</v>
+      </c>
+      <c r="E11" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="79">
+        <v>1000000</v>
+      </c>
+      <c r="O11" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="61">
+        <v>12.5</v>
+      </c>
+      <c r="Q11" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" s="45"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="49">
+        <v>37056</v>
+      </c>
+      <c r="C12" s="50">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="D12" s="45">
+        <v>9898</v>
+      </c>
+      <c r="E12" s="45">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F12" s="45">
+        <f t="shared" si="1"/>
+        <v>-125</v>
+      </c>
+      <c r="I12" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="79">
+        <v>1000000</v>
+      </c>
+      <c r="O12" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" s="61">
+        <v>25</v>
+      </c>
+      <c r="Q12" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="T12" s="45"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="49">
+        <v>37055</v>
+      </c>
+      <c r="C13" s="50">
+        <v>0.98950000000000005</v>
+      </c>
+      <c r="D13" s="45">
+        <v>9903</v>
+      </c>
+      <c r="E13" s="45">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="F13" s="45">
+        <f t="shared" si="1"/>
+        <v>-50</v>
+      </c>
+      <c r="I13" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="92">
+        <v>1000000</v>
+      </c>
+      <c r="O13" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="93">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="T13" s="45"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="49">
+        <v>37054</v>
+      </c>
+      <c r="C14" s="50">
+        <v>0.98940000000000006</v>
+      </c>
+      <c r="D14" s="45">
+        <v>9905</v>
+      </c>
+      <c r="E14" s="45">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F14" s="45">
+        <f t="shared" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="I14" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="85">
+        <v>1000000</v>
+      </c>
+      <c r="O14" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="87">
+        <v>25</v>
+      </c>
+      <c r="Q14" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="T14" s="45"/>
+    </row>
+    <row r="15" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="49">
+        <v>37053</v>
+      </c>
+      <c r="C15" s="50">
+        <v>0.98930000000000007</v>
+      </c>
+      <c r="D15" s="45">
+        <v>9906</v>
+      </c>
+      <c r="E15" s="45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F15" s="45">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="N15" s="80">
+        <v>100000000</v>
+      </c>
+      <c r="O15" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="76">
+        <v>2500</v>
+      </c>
+      <c r="Q15" s="76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B16" s="49">
+        <v>37050</v>
+      </c>
+      <c r="C16" s="50">
+        <v>0.98920000000000008</v>
+      </c>
+      <c r="D16" s="45">
+        <v>9903</v>
+      </c>
+      <c r="E16" s="45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F16" s="45">
+        <f>TickValue*E16</f>
+        <v>75</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="49">
+        <v>37049</v>
+      </c>
+      <c r="C17" s="50">
+        <v>0.98910000000000009</v>
+      </c>
+      <c r="D17" s="45">
+        <v>9900</v>
+      </c>
+      <c r="E17" s="51">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="51">
+        <f>TickValue*E17</f>
+        <v>50</v>
+      </c>
+      <c r="I17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="49">
+        <v>37048</v>
+      </c>
+      <c r="C18" s="50">
+        <f>C17-0.01%</f>
+        <v>0.9890000000000001</v>
+      </c>
+      <c r="D18" s="45">
+        <v>9898</v>
+      </c>
+      <c r="E18" s="53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="53">
+        <f>TickValue*E18</f>
+        <v>25</v>
+      </c>
+      <c r="I18" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="49">
+        <v>37047</v>
+      </c>
+      <c r="C19" s="50">
+        <f t="shared" ref="C19:C22" si="2">C18-0.01%</f>
+        <v>0.98890000000000011</v>
+      </c>
+      <c r="D19" s="45">
+        <v>9897</v>
+      </c>
+      <c r="E19" s="53">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F19" s="53">
+        <f>TickValue*E19</f>
+        <v>-125</v>
+      </c>
+      <c r="I19" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="49">
+        <v>37046</v>
+      </c>
+      <c r="C20" s="50">
+        <f t="shared" si="2"/>
+        <v>0.98880000000000012</v>
+      </c>
+      <c r="D20" s="45">
+        <v>9902</v>
+      </c>
+      <c r="E20" s="53">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="53">
+        <f>TickValue*E20</f>
+        <v>50</v>
+      </c>
+      <c r="I20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="49">
+        <v>37043</v>
+      </c>
+      <c r="C21" s="50">
+        <f t="shared" si="2"/>
+        <v>0.98870000000000013</v>
+      </c>
+      <c r="D21" s="45">
+        <v>9900</v>
+      </c>
+      <c r="E21" s="53">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F21" s="53">
+        <f>TickValue*E21</f>
+        <v>200</v>
+      </c>
+      <c r="I21" s="78" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="49">
+        <v>37042</v>
+      </c>
+      <c r="C22" s="50">
+        <f t="shared" si="2"/>
+        <v>0.98860000000000015</v>
+      </c>
+      <c r="D22" s="45">
+        <v>9892</v>
+      </c>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="I22" s="77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="53"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C24" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="45">
+        <f>D8</f>
+        <v>9900</v>
+      </c>
+      <c r="E24" s="53"/>
+      <c r="F24" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C25" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="45">
+        <f>D22</f>
+        <v>9892</v>
+      </c>
+      <c r="F25" s="53">
+        <f>SUM(F8:F22)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="94">
+        <f>TickValue*(D24-D25)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{B30E80EA-93C9-4138-A8B9-1072B03E19AE}">
+      <formula1>FuturesTickers</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2636,7 +4075,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09AD1A9-5428-4C82-A9BD-6D4983407C24}">
+  <dimension ref="B32:B33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G24"/>
   <sheetViews>
@@ -2681,11 +4142,11 @@
       </c>
       <c r="D5" s="4">
         <f ca="1">2*RAND()*$D$2</f>
-        <v>8.3252073393724153</v>
+        <v>8.5229742365406302</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E14" ca="1" si="0">(1+C5/360*D5/100)</f>
-        <v>1.0002312557594271</v>
+        <v>1.0002367492843482</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>23</v>
@@ -2700,11 +4161,11 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" ref="D6:D14" ca="1" si="1">2*RAND()*$D$2</f>
-        <v>0.28066823268662389</v>
+        <v>9.791294373250448</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0000077963397969</v>
+        <v>1.000271980399257</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -2717,11 +4178,11 @@
       </c>
       <c r="D7" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7901012941726098</v>
+        <v>1.2298939003290676</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002163917026159</v>
+        <v>1.0000341637194536</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -2733,11 +4194,11 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9830141876263507</v>
+        <v>9.477645887298177</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002773059496564</v>
+        <v>1.0002632679413139</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -2749,11 +4210,11 @@
       </c>
       <c r="D9" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7693685519338835</v>
+        <v>7.6151668234907168</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0007307807126611</v>
+        <v>1.0006345972352908</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -2765,11 +4226,11 @@
       </c>
       <c r="D10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6939577381174225</v>
+        <v>2.6865967073791808</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002414988260588</v>
+        <v>1.0000746276863162</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -2781,11 +4242,11 @@
       </c>
       <c r="D11" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3116370531066268</v>
+        <v>8.8690840420059676</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0001753232514752</v>
+        <v>1.0002463634456114</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -2797,11 +4258,11 @@
       </c>
       <c r="D12" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1034367176890729</v>
+        <v>4.8994942378727222</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0002528732421581</v>
+        <v>1.0001360970621631</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -2813,11 +4274,11 @@
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1397890813153619</v>
+        <v>4.7844768748995739</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0001427719189255</v>
+        <v>1.0001329021354139</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -2829,11 +4290,11 @@
       </c>
       <c r="D14" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16712345439670484</v>
+        <v>9.820172786116526</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.000013926954533</v>
+        <v>1.0008183477321764</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2854,11 +4315,11 @@
       </c>
       <c r="D17" s="6">
         <f ca="1">SUMPRODUCT(D5:D14,C5:C14)/C17</f>
-        <v>5.8883776902198752</v>
+        <v>7.3262485063141058</v>
       </c>
       <c r="E17" s="6">
         <f ca="1">(PRODUCT(E5:E15)-1)*(360/C17)*100</f>
-        <v>5.8939848959940839</v>
+        <v>7.3349224113403082</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -2901,11 +4362,11 @@
       </c>
       <c r="D23" s="6">
         <f ca="1">100-D17</f>
-        <v>94.111622309780131</v>
+        <v>92.673751493685899</v>
       </c>
       <c r="E23" s="6">
         <f ca="1">100-E17</f>
-        <v>94.10601510400592</v>
+        <v>92.665077588659699</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>

</xml_diff>